<commit_message>
some changes to recovery bulkhead
</commit_message>
<xml_diff>
--- a/Recovery/Black Powder - Shear Pin Calculator Rev4.xlsx
+++ b/Recovery/Black Powder - Shear Pin Calculator Rev4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Bald-Guy-From-Die-Hard\Recovery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{23B94123-F525-4646-B97E-92602EEF5677}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{CD158C81-2906-4075-8E63-8348033B27FE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1296" yWindow="0" windowWidth="16284" windowHeight="6108" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2592" yWindow="0" windowWidth="16284" windowHeight="6108" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Altimeter Vent Size" sheetId="6" r:id="rId1"/>
@@ -597,6 +597,7 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -627,7 +628,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1389,11 +1389,11 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="38"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
@@ -1432,11 +1432,11 @@
       <c r="F5" s="17"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="37"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="38"/>
       <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1500,11 +1500,11 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
@@ -1539,7 +1539,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1555,20 +1555,20 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="41"/>
+      <c r="C3" s="42"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
@@ -1586,7 +1586,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="29">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>16</v>
@@ -1639,7 +1639,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="28"/>
     </row>
@@ -1648,18 +1648,18 @@
         <v>29</v>
       </c>
       <c r="B11" s="29">
-        <v>1.77</v>
+        <v>3.2</v>
       </c>
       <c r="C11" s="28" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
       <c r="F12" s="16"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1692,7 +1692,7 @@
       </c>
       <c r="B15" s="31">
         <f>B11/454*22.16*12*3307/(3.14159*(B4/2)^2*B5)</f>
-        <v>9.3275426370061663</v>
+        <v>13.701475060009059</v>
       </c>
       <c r="C15" s="28" t="s">
         <v>20</v>
@@ -1716,7 +1716,7 @@
       </c>
       <c r="B17" s="31">
         <f>B10*VLOOKUP(B9,'Screw Shear Strength'!A5:E10,4,FALSE)</f>
-        <v>199.34338566815998</v>
+        <v>149.50753925111999</v>
       </c>
       <c r="C17" s="28" t="s">
         <v>18</v>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="B18" s="31">
         <f>B10*VLOOKUP(B9,'Screw Shear Strength'!A5:E10,5,FALSE)+B8</f>
-        <v>223.03182807454999</v>
+        <v>168.52387105591248</v>
       </c>
       <c r="C18" s="28" t="s">
         <v>18</v>
@@ -1746,7 +1746,7 @@
       </c>
       <c r="B19" s="31">
         <f>B15*3.14159*(B4/2)^2+B8</f>
-        <v>268.72983205692981</v>
+        <v>392.39975330396476</v>
       </c>
       <c r="C19" s="28" t="s">
         <v>18</v>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="B20" s="31">
         <f>B19+B16</f>
-        <v>397.53873697298246</v>
+        <v>521.20865822001747</v>
       </c>
       <c r="C20" s="28" t="s">
         <v>18</v>
@@ -1778,14 +1778,14 @@
       <c r="C21" s="22"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="36" t="s">
         <v>91</v>
       </c>
       <c r="B22">
         <f>5*B11</f>
-        <v>8.85</v>
-      </c>
-      <c r="C22" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="36" t="s">
         <v>19</v>
       </c>
       <c r="D22" t="s">
@@ -1868,11 +1868,11 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
       <c r="D2" s="10" t="s">
         <v>7</v>
       </c>
@@ -1881,9 +1881,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="11">
         <v>9600</v>
       </c>
@@ -1901,10 +1901,10 @@
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="42"/>
+      <c r="E4" s="43"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -2034,17 +2034,17 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="45"/>
       <c r="D17" s="18"/>
-      <c r="E17" s="45" t="s">
+      <c r="E17" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
     </row>
     <row r="18" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">

</xml_diff>